<commit_message>
Last update at night 2:23am
</commit_message>
<xml_diff>
--- a/result/result_1.1.0.0.xlsx
+++ b/result/result_1.1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\version_control_projects\Braille-to-Text-Translator\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14462966-7FF4-4960-BD3F-2BB1F40A189C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C5076A-4741-47F0-BC2A-2ED143559168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,6 +161,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:E118"/>
+  <dimension ref="A4:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="1">
-        <f>MIN($C5:$D5)/MAX($C5:$D5)*100</f>
+        <f t="shared" ref="E5:E36" si="0">MIN($C5:$D5)/MAX($C5:$D5)*100</f>
         <v>95.238095238095227</v>
       </c>
     </row>
@@ -507,7 +510,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="1">
-        <f>MIN($C6:$D6)/MAX($C6:$D6)*100</f>
+        <f t="shared" si="0"/>
         <v>94.73684210526315</v>
       </c>
     </row>
@@ -525,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="1">
-        <f>MIN($C7:$D7)/MAX($C7:$D7)*100</f>
+        <f t="shared" si="0"/>
         <v>85.714285714285708</v>
       </c>
     </row>
@@ -543,7 +546,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="1">
-        <f>MIN($C8:$D8)/MAX($C8:$D8)*100</f>
+        <f t="shared" si="0"/>
         <v>94.117647058823522</v>
       </c>
     </row>
@@ -561,7 +564,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="2">
-        <f>MIN($C9:$D9)/MAX($C9:$D9)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -579,7 +582,7 @@
         <v>21</v>
       </c>
       <c r="E10" s="2">
-        <f>MIN($C10:$D10)/MAX($C10:$D10)*100</f>
+        <f t="shared" si="0"/>
         <v>95.454545454545453</v>
       </c>
     </row>
@@ -597,7 +600,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="2">
-        <f>MIN($C11:$D11)/MAX($C11:$D11)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -615,7 +618,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="2">
-        <f>MIN($C12:$D12)/MAX($C12:$D12)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -633,7 +636,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="2">
-        <f>MIN($C13:$D13)/MAX($C13:$D13)*100</f>
+        <f t="shared" si="0"/>
         <v>94.444444444444443</v>
       </c>
     </row>
@@ -651,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="2">
-        <f>MIN($C14:$D14)/MAX($C14:$D14)*100</f>
+        <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
     </row>
@@ -669,7 +672,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="2">
-        <f>MIN($C15:$D15)/MAX($C15:$D15)*100</f>
+        <f t="shared" si="0"/>
         <v>94.444444444444443</v>
       </c>
     </row>
@@ -687,7 +690,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="2">
-        <f>MIN($C16:$D16)/MAX($C16:$D16)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -707,7 +710,7 @@
         <v>180</v>
       </c>
       <c r="E17" s="4">
-        <f>MIN($C17:$D17)/MAX($C17:$D17)*100</f>
+        <f t="shared" si="0"/>
         <v>95.744680851063833</v>
       </c>
     </row>
@@ -725,7 +728,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="2">
-        <f>MIN($C18:$D18)/MAX($C18:$D18)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -743,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="2">
-        <f>MIN($C19:$D19)/MAX($C19:$D19)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -761,7 +764,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="2">
-        <f>MIN($C20:$D20)/MAX($C20:$D20)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -779,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="2">
-        <f>MIN($C21:$D21)/MAX($C21:$D21)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -797,7 +800,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="2">
-        <f>MIN($C22:$D22)/MAX($C22:$D22)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -817,7 +820,7 @@
         <v>73</v>
       </c>
       <c r="E23" s="4">
-        <f>MIN($C23:$D23)/MAX($C23:$D23)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -835,7 +838,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="2">
-        <f>MIN($C24:$D24)/MAX($C24:$D24)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -853,7 +856,7 @@
         <v>14</v>
       </c>
       <c r="E25" s="2">
-        <f>MIN($C25:$D25)/MAX($C25:$D25)*100</f>
+        <f t="shared" si="0"/>
         <v>93.333333333333329</v>
       </c>
     </row>
@@ -871,7 +874,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="2">
-        <f>MIN($C26:$D26)/MAX($C26:$D26)*100</f>
+        <f t="shared" si="0"/>
         <v>94.444444444444443</v>
       </c>
     </row>
@@ -889,7 +892,7 @@
         <v>16</v>
       </c>
       <c r="E27" s="2">
-        <f>MIN($C27:$D27)/MAX($C27:$D27)*100</f>
+        <f t="shared" si="0"/>
         <v>94.117647058823522</v>
       </c>
     </row>
@@ -907,7 +910,7 @@
         <v>19</v>
       </c>
       <c r="E28" s="2">
-        <f>MIN($C28:$D28)/MAX($C28:$D28)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -925,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="2">
-        <f>MIN($C29:$D29)/MAX($C29:$D29)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -943,7 +946,7 @@
         <v>18</v>
       </c>
       <c r="E30" s="2">
-        <f>MIN($C30:$D30)/MAX($C30:$D30)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -961,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="E31" s="2">
-        <f>MIN($C31:$D31)/MAX($C31:$D31)*100</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
@@ -979,7 +982,7 @@
         <v>14</v>
       </c>
       <c r="E32" s="2">
-        <f>MIN($C32:$D32)/MAX($C32:$D32)*100</f>
+        <f t="shared" si="0"/>
         <v>93.333333333333329</v>
       </c>
     </row>
@@ -997,7 +1000,7 @@
         <v>19</v>
       </c>
       <c r="E33" s="2">
-        <f>MIN($C33:$D33)/MAX($C33:$D33)*100</f>
+        <f t="shared" si="0"/>
         <v>86.36363636363636</v>
       </c>
     </row>
@@ -1015,7 +1018,7 @@
         <v>13</v>
       </c>
       <c r="E34" s="2">
-        <f>MIN($C34:$D34)/MAX($C34:$D34)*100</f>
+        <f t="shared" si="0"/>
         <v>86.666666666666671</v>
       </c>
     </row>
@@ -1035,7 +1038,7 @@
         <v>165</v>
       </c>
       <c r="E35" s="4">
-        <f>MIN($C35:$D35)/MAX($C35:$D35)*100</f>
+        <f t="shared" si="0"/>
         <v>94.285714285714278</v>
       </c>
     </row>
@@ -1053,7 +1056,7 @@
         <v>13</v>
       </c>
       <c r="E36" s="2">
-        <f>MIN($C36:$D36)/MAX($C36:$D36)*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -1071,7 +1074,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="2">
-        <f>MIN($C37:$D37)/MAX($C37:$D37)*100</f>
+        <f t="shared" ref="E37:E68" si="1">MIN($C37:$D37)/MAX($C37:$D37)*100</f>
         <v>100</v>
       </c>
     </row>
@@ -1089,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="E38" s="2">
-        <f>MIN($C38:$D38)/MAX($C38:$D38)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1107,7 +1110,7 @@
         <v>14</v>
       </c>
       <c r="E39" s="2">
-        <f>MIN($C39:$D39)/MAX($C39:$D39)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1125,7 +1128,7 @@
         <v>18</v>
       </c>
       <c r="E40" s="2">
-        <f>MIN($C40:$D40)/MAX($C40:$D40)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1143,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="2">
-        <f>MIN($C41:$D41)/MAX($C41:$D41)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1161,7 +1164,7 @@
         <v>13</v>
       </c>
       <c r="E42" s="2">
-        <f>MIN($C42:$D42)/MAX($C42:$D42)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1179,7 +1182,7 @@
         <v>16</v>
       </c>
       <c r="E43" s="2">
-        <f>MIN($C43:$D43)/MAX($C43:$D43)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1197,7 +1200,7 @@
         <v>9</v>
       </c>
       <c r="E44" s="2">
-        <f>MIN($C44:$D44)/MAX($C44:$D44)*100</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
@@ -1217,7 +1220,7 @@
         <v>103</v>
       </c>
       <c r="E45" s="4">
-        <f>MIN($C45:$D45)/MAX($C45:$D45)*100</f>
+        <f t="shared" si="1"/>
         <v>99.038461538461547</v>
       </c>
     </row>
@@ -1235,7 +1238,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2">
-        <f>MIN($C46:$D46)/MAX($C46:$D46)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1253,7 +1256,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="2">
-        <f>MIN($C47:$D47)/MAX($C47:$D47)*100</f>
+        <f t="shared" si="1"/>
         <v>88.888888888888886</v>
       </c>
     </row>
@@ -1271,7 +1274,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="2">
-        <f>MIN($C48:$D48)/MAX($C48:$D48)*100</f>
+        <f t="shared" si="1"/>
         <v>93.75</v>
       </c>
     </row>
@@ -1289,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="E49" s="2">
-        <f>MIN($C49:$D49)/MAX($C49:$D49)*100</f>
+        <f t="shared" si="1"/>
         <v>90.476190476190482</v>
       </c>
     </row>
@@ -1307,7 +1310,7 @@
         <v>16</v>
       </c>
       <c r="E50" s="2">
-        <f>MIN($C50:$D50)/MAX($C50:$D50)*100</f>
+        <f t="shared" si="1"/>
         <v>94.117647058823522</v>
       </c>
     </row>
@@ -1325,7 +1328,7 @@
         <v>12</v>
       </c>
       <c r="E51" s="2">
-        <f>MIN($C51:$D51)/MAX($C51:$D51)*100</f>
+        <f t="shared" si="1"/>
         <v>85.714285714285708</v>
       </c>
     </row>
@@ -1343,7 +1346,7 @@
         <v>14</v>
       </c>
       <c r="E52" s="2">
-        <f>MIN($C52:$D52)/MAX($C52:$D52)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1361,7 +1364,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="2">
-        <f>MIN($C53:$D53)/MAX($C53:$D53)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1379,7 +1382,7 @@
         <v>13</v>
       </c>
       <c r="E54" s="2">
-        <f>MIN($C54:$D54)/MAX($C54:$D54)*100</f>
+        <f t="shared" si="1"/>
         <v>86.666666666666671</v>
       </c>
     </row>
@@ -1397,7 +1400,7 @@
         <v>14</v>
       </c>
       <c r="E55" s="2">
-        <f>MIN($C55:$D55)/MAX($C55:$D55)*100</f>
+        <f t="shared" si="1"/>
         <v>93.333333333333329</v>
       </c>
     </row>
@@ -1415,7 +1418,7 @@
         <v>12</v>
       </c>
       <c r="E56" s="2">
-        <f>MIN($C56:$D56)/MAX($C56:$D56)*100</f>
+        <f t="shared" si="1"/>
         <v>92.307692307692307</v>
       </c>
     </row>
@@ -1435,7 +1438,7 @@
         <v>151</v>
       </c>
       <c r="E57" s="4">
-        <f>MIN($C57:$D57)/MAX($C57:$D57)*100</f>
+        <f t="shared" si="1"/>
         <v>92.638036809815944</v>
       </c>
     </row>
@@ -1453,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="E58" s="2">
-        <f>MIN($C58:$D58)/MAX($C58:$D58)*100</f>
+        <f t="shared" si="1"/>
         <v>90.909090909090907</v>
       </c>
     </row>
@@ -1471,7 +1474,7 @@
         <v>18</v>
       </c>
       <c r="E59" s="2">
-        <f>MIN($C59:$D59)/MAX($C59:$D59)*100</f>
+        <f t="shared" si="1"/>
         <v>94.73684210526315</v>
       </c>
     </row>
@@ -1489,7 +1492,7 @@
         <v>10</v>
       </c>
       <c r="E60" s="2">
-        <f>MIN($C60:$D60)/MAX($C60:$D60)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1507,7 +1510,7 @@
         <v>18</v>
       </c>
       <c r="E61" s="2">
-        <f>MIN($C61:$D61)/MAX($C61:$D61)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1525,7 +1528,7 @@
         <v>18</v>
       </c>
       <c r="E62" s="2">
-        <f>MIN($C62:$D62)/MAX($C62:$D62)*100</f>
+        <f t="shared" si="1"/>
         <v>94.73684210526315</v>
       </c>
     </row>
@@ -1543,7 +1546,7 @@
         <v>16</v>
       </c>
       <c r="E63" s="2">
-        <f>MIN($C63:$D63)/MAX($C63:$D63)*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -1563,7 +1566,7 @@
         <v>90</v>
       </c>
       <c r="E64" s="4">
-        <f>MIN($C64:$D64)/MAX($C64:$D64)*100</f>
+        <f t="shared" si="1"/>
         <v>96.774193548387103</v>
       </c>
     </row>
@@ -1581,7 +1584,7 @@
         <v>23</v>
       </c>
       <c r="E65" s="2">
-        <f>MIN($C65:$D65)/MAX($C65:$D65)*100</f>
+        <f t="shared" si="1"/>
         <v>95.833333333333343</v>
       </c>
     </row>
@@ -1599,7 +1602,7 @@
         <v>22</v>
       </c>
       <c r="E66" s="2">
-        <f>MIN($C66:$D66)/MAX($C66:$D66)*100</f>
+        <f t="shared" si="1"/>
         <v>91.666666666666657</v>
       </c>
     </row>
@@ -1617,7 +1620,7 @@
         <v>23</v>
       </c>
       <c r="E67" s="2">
-        <f>MIN($C67:$D67)/MAX($C67:$D67)*100</f>
+        <f t="shared" si="1"/>
         <v>95.833333333333343</v>
       </c>
     </row>
@@ -1635,7 +1638,7 @@
         <v>22</v>
       </c>
       <c r="E68" s="2">
-        <f>MIN($C68:$D68)/MAX($C68:$D68)*100</f>
+        <f t="shared" si="1"/>
         <v>95.652173913043484</v>
       </c>
     </row>
@@ -1653,7 +1656,7 @@
         <v>23</v>
       </c>
       <c r="E69" s="2">
-        <f>MIN($C69:$D69)/MAX($C69:$D69)*100</f>
+        <f t="shared" ref="E69:E100" si="2">MIN($C69:$D69)/MAX($C69:$D69)*100</f>
         <v>92</v>
       </c>
     </row>
@@ -1671,7 +1674,7 @@
         <v>14</v>
       </c>
       <c r="E70" s="2">
-        <f>MIN($C70:$D70)/MAX($C70:$D70)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1689,7 +1692,7 @@
         <v>19</v>
       </c>
       <c r="E71" s="2">
-        <f>MIN($C71:$D71)/MAX($C71:$D71)*100</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
@@ -1707,7 +1710,7 @@
         <v>25</v>
       </c>
       <c r="E72" s="2">
-        <f>MIN($C72:$D72)/MAX($C72:$D72)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1725,7 +1728,7 @@
         <v>6</v>
       </c>
       <c r="E73" s="2">
-        <f>MIN($C73:$D73)/MAX($C73:$D73)*100</f>
+        <f t="shared" si="2"/>
         <v>66.666666666666657</v>
       </c>
     </row>
@@ -1745,7 +1748,7 @@
         <v>177</v>
       </c>
       <c r="E74" s="4">
-        <f>MIN($C74:$D74)/MAX($C74:$D74)*100</f>
+        <f t="shared" si="2"/>
         <v>91.709844559585491</v>
       </c>
     </row>
@@ -1763,7 +1766,7 @@
         <v>20</v>
       </c>
       <c r="E75" s="2">
-        <f>MIN($C75:$D75)/MAX($C75:$D75)*100</f>
+        <f t="shared" si="2"/>
         <v>76.923076923076934</v>
       </c>
     </row>
@@ -1781,7 +1784,7 @@
         <v>9</v>
       </c>
       <c r="E76" s="2">
-        <f>MIN($C76:$D76)/MAX($C76:$D76)*100</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
@@ -1799,7 +1802,7 @@
         <v>21</v>
       </c>
       <c r="E77" s="2">
-        <f>MIN($C77:$D77)/MAX($C77:$D77)*100</f>
+        <f t="shared" si="2"/>
         <v>91.304347826086953</v>
       </c>
     </row>
@@ -1817,7 +1820,7 @@
         <v>24</v>
       </c>
       <c r="E78" s="2">
-        <f>MIN($C78:$D78)/MAX($C78:$D78)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1835,7 +1838,7 @@
         <v>23</v>
       </c>
       <c r="E79" s="2">
-        <f>MIN($C79:$D79)/MAX($C79:$D79)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1853,7 +1856,7 @@
         <v>21</v>
       </c>
       <c r="E80" s="2">
-        <f>MIN($C80:$D80)/MAX($C80:$D80)*100</f>
+        <f t="shared" si="2"/>
         <v>95.454545454545453</v>
       </c>
     </row>
@@ -1871,7 +1874,7 @@
         <v>19</v>
       </c>
       <c r="E81" s="2">
-        <f>MIN($C81:$D81)/MAX($C81:$D81)*100</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
     </row>
@@ -1889,7 +1892,7 @@
         <v>6</v>
       </c>
       <c r="E82" s="2">
-        <f>MIN($C82:$D82)/MAX($C82:$D82)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1907,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="E83" s="2">
-        <f>MIN($C83:$D83)/MAX($C83:$D83)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1925,7 +1928,7 @@
         <v>21</v>
       </c>
       <c r="E84" s="2">
-        <f>MIN($C84:$D84)/MAX($C84:$D84)*100</f>
+        <f t="shared" si="2"/>
         <v>91.304347826086953</v>
       </c>
     </row>
@@ -1943,7 +1946,7 @@
         <v>7</v>
       </c>
       <c r="E85" s="2">
-        <f>MIN($C85:$D85)/MAX($C85:$D85)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1963,7 +1966,7 @@
         <v>191</v>
       </c>
       <c r="E86" s="4">
-        <f>MIN($C86:$D86)/MAX($C86:$D86)*100</f>
+        <f t="shared" si="2"/>
         <v>93.627450980392155</v>
       </c>
     </row>
@@ -1981,7 +1984,7 @@
         <v>26</v>
       </c>
       <c r="E87" s="2">
-        <f>MIN($C87:$D87)/MAX($C87:$D87)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -1999,7 +2002,7 @@
         <v>19</v>
       </c>
       <c r="E88" s="2">
-        <f>MIN($C88:$D88)/MAX($C88:$D88)*100</f>
+        <f t="shared" si="2"/>
         <v>86.36363636363636</v>
       </c>
     </row>
@@ -2017,7 +2020,7 @@
         <v>10</v>
       </c>
       <c r="E89" s="2">
-        <f>MIN($C89:$D89)/MAX($C89:$D89)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2035,7 +2038,7 @@
         <v>19</v>
       </c>
       <c r="E90" s="2">
-        <f>MIN($C90:$D90)/MAX($C90:$D90)*100</f>
+        <f t="shared" si="2"/>
         <v>90.476190476190482</v>
       </c>
     </row>
@@ -2053,7 +2056,7 @@
         <v>21</v>
       </c>
       <c r="E91" s="2">
-        <f>MIN($C91:$D91)/MAX($C91:$D91)*100</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
     </row>
@@ -2071,7 +2074,7 @@
         <v>19</v>
       </c>
       <c r="E92" s="2">
-        <f>MIN($C92:$D92)/MAX($C92:$D92)*100</f>
+        <f t="shared" si="2"/>
         <v>90.476190476190482</v>
       </c>
     </row>
@@ -2089,7 +2092,7 @@
         <v>24</v>
       </c>
       <c r="E93" s="2">
-        <f>MIN($C93:$D93)/MAX($C93:$D93)*100</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
     </row>
@@ -2107,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="E94" s="2">
-        <f>MIN($C94:$D94)/MAX($C94:$D94)*100</f>
+        <f t="shared" si="2"/>
         <v>83.333333333333343</v>
       </c>
     </row>
@@ -2125,7 +2128,7 @@
         <v>17</v>
       </c>
       <c r="E95" s="2">
-        <f>MIN($C95:$D95)/MAX($C95:$D95)*100</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
@@ -2143,7 +2146,7 @@
         <v>17</v>
       </c>
       <c r="E96" s="2">
-        <f>MIN($C96:$D96)/MAX($C96:$D96)*100</f>
+        <f t="shared" si="2"/>
         <v>89.473684210526315</v>
       </c>
     </row>
@@ -2163,7 +2166,7 @@
         <v>177</v>
       </c>
       <c r="E97" s="4">
-        <f>MIN($C97:$D97)/MAX($C97:$D97)*100</f>
+        <f t="shared" si="2"/>
         <v>90.769230769230774</v>
       </c>
     </row>
@@ -2181,7 +2184,7 @@
         <v>23</v>
       </c>
       <c r="E98" s="2">
-        <f>MIN($C98:$D98)/MAX($C98:$D98)*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -2199,7 +2202,7 @@
         <v>22</v>
       </c>
       <c r="E99" s="2">
-        <f>MIN($C99:$D99)/MAX($C99:$D99)*100</f>
+        <f t="shared" si="2"/>
         <v>95.652173913043484</v>
       </c>
     </row>
@@ -2217,7 +2220,7 @@
         <v>21</v>
       </c>
       <c r="E100" s="2">
-        <f>MIN($C100:$D100)/MAX($C100:$D100)*100</f>
+        <f t="shared" si="2"/>
         <v>95.454545454545453</v>
       </c>
     </row>
@@ -2235,7 +2238,7 @@
         <v>25</v>
       </c>
       <c r="E101" s="2">
-        <f>MIN($C101:$D101)/MAX($C101:$D101)*100</f>
+        <f t="shared" ref="E101:E118" si="3">MIN($C101:$D101)/MAX($C101:$D101)*100</f>
         <v>100</v>
       </c>
     </row>
@@ -2253,7 +2256,7 @@
         <v>11</v>
       </c>
       <c r="E102" s="2">
-        <f>MIN($C102:$D102)/MAX($C102:$D102)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2271,7 +2274,7 @@
         <v>21</v>
       </c>
       <c r="E103" s="2">
-        <f>MIN($C103:$D103)/MAX($C103:$D103)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2289,7 +2292,7 @@
         <v>11</v>
       </c>
       <c r="E104" s="2">
-        <f>MIN($C104:$D104)/MAX($C104:$D104)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2307,7 +2310,7 @@
         <v>20</v>
       </c>
       <c r="E105" s="2">
-        <f>MIN($C105:$D105)/MAX($C105:$D105)*100</f>
+        <f t="shared" si="3"/>
         <v>95.238095238095227</v>
       </c>
     </row>
@@ -2325,7 +2328,7 @@
         <v>19</v>
       </c>
       <c r="E106" s="2">
-        <f>MIN($C106:$D106)/MAX($C106:$D106)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2345,7 +2348,7 @@
         <v>173</v>
       </c>
       <c r="E107" s="4">
-        <f>MIN($C107:$D107)/MAX($C107:$D107)*100</f>
+        <f t="shared" si="3"/>
         <v>98.295454545454547</v>
       </c>
     </row>
@@ -2363,7 +2366,7 @@
         <v>20</v>
       </c>
       <c r="E108" s="2">
-        <f>MIN($C108:$D108)/MAX($C108:$D108)*100</f>
+        <f t="shared" si="3"/>
         <v>95.238095238095227</v>
       </c>
     </row>
@@ -2381,7 +2384,7 @@
         <v>23</v>
       </c>
       <c r="E109" s="2">
-        <f>MIN($C109:$D109)/MAX($C109:$D109)*100</f>
+        <f t="shared" si="3"/>
         <v>95.833333333333343</v>
       </c>
     </row>
@@ -2399,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E110" s="2">
-        <f>MIN($C110:$D110)/MAX($C110:$D110)*100</f>
+        <f t="shared" si="3"/>
         <v>83.333333333333343</v>
       </c>
     </row>
@@ -2417,7 +2420,7 @@
         <v>21</v>
       </c>
       <c r="E111" s="2">
-        <f>MIN($C111:$D111)/MAX($C111:$D111)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2435,7 +2438,7 @@
         <v>12</v>
       </c>
       <c r="E112" s="2">
-        <f>MIN($C112:$D112)/MAX($C112:$D112)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2453,7 +2456,7 @@
         <v>25</v>
       </c>
       <c r="E113" s="2">
-        <f>MIN($C113:$D113)/MAX($C113:$D113)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2471,7 +2474,7 @@
         <v>21</v>
       </c>
       <c r="E114" s="2">
-        <f>MIN($C114:$D114)/MAX($C114:$D114)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2489,7 +2492,7 @@
         <v>22</v>
       </c>
       <c r="E115" s="2">
-        <f>MIN($C115:$D115)/MAX($C115:$D115)*100</f>
+        <f t="shared" si="3"/>
         <v>91.666666666666657</v>
       </c>
     </row>
@@ -2507,7 +2510,7 @@
         <v>4</v>
       </c>
       <c r="E116" s="2">
-        <f>MIN($C116:$D116)/MAX($C116:$D116)*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -2525,7 +2528,7 @@
         <v>16</v>
       </c>
       <c r="E117" s="2">
-        <f>MIN($C117:$D117)/MAX($C117:$D117)*100</f>
+        <f t="shared" si="3"/>
         <v>94.117647058823522</v>
       </c>
     </row>
@@ -2545,8 +2548,22 @@
         <v>174</v>
       </c>
       <c r="E118" s="4">
-        <f>MIN($C118:$D118)/MAX($C118:$D118)*100</f>
+        <f t="shared" si="3"/>
         <v>96.132596685082873</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C124" s="2">
+        <f>SUM(C17,C23, C35,C45,C57,C64,C74,C86,C97,C107,C118)</f>
+        <v>1745</v>
+      </c>
+      <c r="D124" s="7">
+        <f>SUM(D17,D23, D35,D45,D57,D64,D74,D86,D97,D107,D118)</f>
+        <v>1654</v>
+      </c>
+      <c r="E124" s="2">
+        <f t="shared" ref="E124" si="4">MIN($C124:$D124)/MAX($C124:$D124)*100</f>
+        <v>94.785100286532952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>